<commit_message>
fixed view sheet issues (sequencing)
</commit_message>
<xml_diff>
--- a/InputSheet/Input Sheet-PA tool.xlsx
+++ b/InputSheet/Input Sheet-PA tool.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>BSE Code</t>
   </si>
@@ -202,18 +202,6 @@
   </si>
   <si>
     <t>FY 13/14</t>
-  </si>
-  <si>
-    <t>Net Profit(In Cr)</t>
-  </si>
-  <si>
-    <t>Audit Fee (In Cr)</t>
-  </si>
-  <si>
-    <t>Audit Related Fee (In Cr)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non Audit Fee </t>
   </si>
   <si>
     <t>CSR Committee Attendance</t>
@@ -310,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,13 +325,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,7 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -487,20 +487,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -516,10 +506,81 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -527,42 +588,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -847,17 +873,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ240"/>
+  <dimension ref="A1:AJ241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="C240" sqref="C240:G240"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="J218" sqref="J218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="35" customWidth="1"/>
-    <col min="3" max="9" width="16.28515625" style="31"/>
+    <col min="2" max="2" width="36.5703125" style="31" customWidth="1"/>
+    <col min="3" max="9" width="16.28515625" style="29"/>
     <col min="10" max="20" width="16.28515625" style="14"/>
     <col min="21" max="21" width="28.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="22" max="27" width="16.28515625" style="14"/>
@@ -874,7 +900,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P1" s="4"/>
     </row>
@@ -882,7 +908,7 @@
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
@@ -958,15 +984,15 @@
       <c r="AA2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
     </row>
     <row r="3" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A3" s="2"/>
@@ -996,15 +1022,15 @@
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
       <c r="AA3" s="12"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
     </row>
     <row r="4" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A4" s="2"/>
@@ -1034,15 +1060,15 @@
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
       <c r="AA4" s="12"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="39"/>
+      <c r="AE4" s="39"/>
+      <c r="AF4" s="39"/>
+      <c r="AG4" s="39"/>
+      <c r="AH4" s="40"/>
+      <c r="AI4" s="39"/>
+      <c r="AJ4" s="39"/>
     </row>
     <row r="5" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A5" s="2"/>
@@ -1072,15 +1098,15 @@
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2"/>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
+      <c r="AB5" s="39"/>
+      <c r="AC5" s="40"/>
+      <c r="AD5" s="39"/>
+      <c r="AE5" s="39"/>
+      <c r="AF5" s="39"/>
+      <c r="AG5" s="39"/>
+      <c r="AH5" s="40"/>
+      <c r="AI5" s="39"/>
+      <c r="AJ5" s="39"/>
     </row>
     <row r="6" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A6" s="2"/>
@@ -1110,15 +1136,15 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="12"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="40"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="39"/>
+      <c r="AH6" s="40"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="39"/>
     </row>
     <row r="7" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A7" s="2"/>
@@ -1148,15 +1174,15 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="12"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="12"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
+      <c r="AB7" s="39"/>
+      <c r="AC7" s="40"/>
+      <c r="AD7" s="39"/>
+      <c r="AE7" s="39"/>
+      <c r="AF7" s="39"/>
+      <c r="AG7" s="39"/>
+      <c r="AH7" s="40"/>
+      <c r="AI7" s="39"/>
+      <c r="AJ7" s="39"/>
     </row>
     <row r="8" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A8" s="2"/>
@@ -1186,15 +1212,15 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="40"/>
+      <c r="AD8" s="39"/>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="39"/>
+      <c r="AH8" s="40"/>
+      <c r="AI8" s="39"/>
+      <c r="AJ8" s="39"/>
     </row>
     <row r="9" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A9" s="2"/>
@@ -1224,15 +1250,15 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
       <c r="AA9" s="12"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="12"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="12"/>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="2"/>
+      <c r="AB9" s="39"/>
+      <c r="AC9" s="40"/>
+      <c r="AD9" s="39"/>
+      <c r="AE9" s="39"/>
+      <c r="AF9" s="39"/>
+      <c r="AG9" s="39"/>
+      <c r="AH9" s="40"/>
+      <c r="AI9" s="39"/>
+      <c r="AJ9" s="39"/>
     </row>
     <row r="10" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A10" s="2"/>
@@ -1262,15 +1288,15 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
       <c r="AA10" s="12"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="12"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="12"/>
-      <c r="AI10" s="2"/>
-      <c r="AJ10" s="2"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="40"/>
+      <c r="AD10" s="39"/>
+      <c r="AE10" s="39"/>
+      <c r="AF10" s="39"/>
+      <c r="AG10" s="39"/>
+      <c r="AH10" s="40"/>
+      <c r="AI10" s="39"/>
+      <c r="AJ10" s="39"/>
     </row>
     <row r="11" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="2"/>
@@ -1300,15 +1326,15 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="12"/>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
+      <c r="AB11" s="39"/>
+      <c r="AC11" s="40"/>
+      <c r="AD11" s="39"/>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="39"/>
+      <c r="AG11" s="39"/>
+      <c r="AH11" s="40"/>
+      <c r="AI11" s="39"/>
+      <c r="AJ11" s="39"/>
     </row>
     <row r="12" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A12" s="2"/>
@@ -1338,15 +1364,15 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="12"/>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="40"/>
+      <c r="AD12" s="39"/>
+      <c r="AE12" s="39"/>
+      <c r="AF12" s="39"/>
+      <c r="AG12" s="39"/>
+      <c r="AH12" s="40"/>
+      <c r="AI12" s="39"/>
+      <c r="AJ12" s="39"/>
     </row>
     <row r="13" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A13" s="2"/>
@@ -1376,15 +1402,15 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="40"/>
+      <c r="AD13" s="39"/>
+      <c r="AE13" s="39"/>
+      <c r="AF13" s="39"/>
+      <c r="AG13" s="39"/>
+      <c r="AH13" s="40"/>
+      <c r="AI13" s="39"/>
+      <c r="AJ13" s="39"/>
     </row>
     <row r="14" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A14" s="2"/>
@@ -1414,15 +1440,15 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
       <c r="AA14" s="12"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="12"/>
-      <c r="AI14" s="2"/>
-      <c r="AJ14" s="2"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="40"/>
+      <c r="AD14" s="39"/>
+      <c r="AE14" s="39"/>
+      <c r="AF14" s="39"/>
+      <c r="AG14" s="39"/>
+      <c r="AH14" s="40"/>
+      <c r="AI14" s="39"/>
+      <c r="AJ14" s="39"/>
     </row>
     <row r="15" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A15" s="2"/>
@@ -1452,15 +1478,15 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="12"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="12"/>
-      <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
+      <c r="AB15" s="39"/>
+      <c r="AC15" s="40"/>
+      <c r="AD15" s="39"/>
+      <c r="AE15" s="39"/>
+      <c r="AF15" s="39"/>
+      <c r="AG15" s="39"/>
+      <c r="AH15" s="40"/>
+      <c r="AI15" s="39"/>
+      <c r="AJ15" s="39"/>
     </row>
     <row r="16" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A16" s="2"/>
@@ -1490,15 +1516,15 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="12"/>
-      <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="12"/>
-      <c r="AI16" s="2"/>
-      <c r="AJ16" s="2"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="40"/>
+      <c r="AD16" s="39"/>
+      <c r="AE16" s="39"/>
+      <c r="AF16" s="39"/>
+      <c r="AG16" s="39"/>
+      <c r="AH16" s="40"/>
+      <c r="AI16" s="39"/>
+      <c r="AJ16" s="39"/>
     </row>
     <row r="17" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A17" s="2"/>
@@ -1528,15 +1554,15 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="12"/>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
+      <c r="AB17" s="39"/>
+      <c r="AC17" s="40"/>
+      <c r="AD17" s="39"/>
+      <c r="AE17" s="39"/>
+      <c r="AF17" s="39"/>
+      <c r="AG17" s="39"/>
+      <c r="AH17" s="40"/>
+      <c r="AI17" s="39"/>
+      <c r="AJ17" s="39"/>
     </row>
     <row r="18" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A18" s="2"/>
@@ -1566,15 +1592,15 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="12"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="12"/>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
+      <c r="AB18" s="39"/>
+      <c r="AC18" s="40"/>
+      <c r="AD18" s="39"/>
+      <c r="AE18" s="39"/>
+      <c r="AF18" s="39"/>
+      <c r="AG18" s="39"/>
+      <c r="AH18" s="40"/>
+      <c r="AI18" s="39"/>
+      <c r="AJ18" s="39"/>
     </row>
     <row r="19" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A19" s="2"/>
@@ -1604,15 +1630,15 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="2"/>
-      <c r="AH19" s="12"/>
-      <c r="AI19" s="2"/>
-      <c r="AJ19" s="2"/>
+      <c r="AB19" s="39"/>
+      <c r="AC19" s="40"/>
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="39"/>
+      <c r="AF19" s="39"/>
+      <c r="AG19" s="39"/>
+      <c r="AH19" s="40"/>
+      <c r="AI19" s="39"/>
+      <c r="AJ19" s="39"/>
     </row>
     <row r="20" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="2"/>
@@ -1642,15 +1668,15 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="12"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="12"/>
-      <c r="AI20" s="2"/>
-      <c r="AJ20" s="2"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="40"/>
+      <c r="AD20" s="39"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="39"/>
+      <c r="AG20" s="39"/>
+      <c r="AH20" s="40"/>
+      <c r="AI20" s="39"/>
+      <c r="AJ20" s="39"/>
     </row>
     <row r="21" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A21" s="2"/>
@@ -1680,15 +1706,15 @@
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="12"/>
-      <c r="AD21" s="2"/>
-      <c r="AE21" s="2"/>
-      <c r="AF21" s="2"/>
-      <c r="AG21" s="2"/>
-      <c r="AH21" s="12"/>
-      <c r="AI21" s="2"/>
-      <c r="AJ21" s="2"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="40"/>
+      <c r="AD21" s="39"/>
+      <c r="AE21" s="39"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="39"/>
+      <c r="AH21" s="40"/>
+      <c r="AI21" s="39"/>
+      <c r="AJ21" s="39"/>
     </row>
     <row r="22" spans="1:36" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="2"/>
@@ -1718,21 +1744,21 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
       <c r="AA22" s="12"/>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="12"/>
-      <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
-      <c r="AG22" s="2"/>
-      <c r="AH22" s="12"/>
-      <c r="AI22" s="2"/>
-      <c r="AJ22" s="2"/>
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="40"/>
+      <c r="AD22" s="39"/>
+      <c r="AE22" s="39"/>
+      <c r="AF22" s="39"/>
+      <c r="AG22" s="39"/>
+      <c r="AH22" s="40"/>
+      <c r="AI22" s="39"/>
+      <c r="AJ22" s="39"/>
     </row>
     <row r="23" spans="1:36" ht="25.5">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="13" t="s">
         <v>28</v>
       </c>
@@ -2091,7 +2117,7 @@
       <c r="A44" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="33" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="13" t="s">
@@ -2414,7 +2440,7 @@
       <c r="A65" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="32" t="s">
         <v>42</v>
       </c>
       <c r="C65" s="13" t="s">
@@ -2799,7 +2825,7 @@
       <c r="A86" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B86" s="36"/>
+      <c r="B86" s="32"/>
       <c r="C86" s="13" t="s">
         <v>43</v>
       </c>
@@ -3182,7 +3208,7 @@
       <c r="A107" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B107" s="36"/>
+      <c r="B107" s="32"/>
       <c r="C107" s="13" t="s">
         <v>43</v>
       </c>
@@ -3306,7 +3332,8 @@
       <c r="M112" s="23"/>
       <c r="N112" s="23"/>
     </row>
-    <row r="113" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="113" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A113" s="14"/>
       <c r="B113" s="6" t="str">
         <v/>
       </c>
@@ -3323,7 +3350,8 @@
       <c r="M113" s="23"/>
       <c r="N113" s="23"/>
     </row>
-    <row r="114" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="114" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A114" s="14"/>
       <c r="B114" s="6" t="str">
         <v/>
       </c>
@@ -3340,7 +3368,8 @@
       <c r="M114" s="23"/>
       <c r="N114" s="23"/>
     </row>
-    <row r="115" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="115" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A115" s="14"/>
       <c r="B115" s="6" t="str">
         <v/>
       </c>
@@ -3357,7 +3386,8 @@
       <c r="M115" s="23"/>
       <c r="N115" s="23"/>
     </row>
-    <row r="116" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="116" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A116" s="14"/>
       <c r="B116" s="6" t="str">
         <v/>
       </c>
@@ -3374,7 +3404,8 @@
       <c r="M116" s="23"/>
       <c r="N116" s="23"/>
     </row>
-    <row r="117" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="117" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A117" s="14"/>
       <c r="B117" s="6" t="str">
         <v/>
       </c>
@@ -3391,7 +3422,8 @@
       <c r="M117" s="23"/>
       <c r="N117" s="23"/>
     </row>
-    <row r="118" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="118" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A118" s="14"/>
       <c r="B118" s="6" t="str">
         <v/>
       </c>
@@ -3408,7 +3440,8 @@
       <c r="M118" s="23"/>
       <c r="N118" s="23"/>
     </row>
-    <row r="119" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="119" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A119" s="14"/>
       <c r="B119" s="6" t="str">
         <v/>
       </c>
@@ -3425,7 +3458,8 @@
       <c r="M119" s="23"/>
       <c r="N119" s="23"/>
     </row>
-    <row r="120" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="120" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A120" s="14"/>
       <c r="B120" s="6" t="str">
         <v/>
       </c>
@@ -3442,7 +3476,8 @@
       <c r="M120" s="23"/>
       <c r="N120" s="23"/>
     </row>
-    <row r="121" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="121" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A121" s="14"/>
       <c r="B121" s="6" t="str">
         <v/>
       </c>
@@ -3459,7 +3494,8 @@
       <c r="M121" s="23"/>
       <c r="N121" s="23"/>
     </row>
-    <row r="122" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="122" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A122" s="14"/>
       <c r="B122" s="24" t="str">
         <v/>
       </c>
@@ -3476,7 +3512,8 @@
       <c r="M122" s="23"/>
       <c r="N122" s="23"/>
     </row>
-    <row r="123" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="123" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A123" s="14"/>
       <c r="B123" s="6" t="str">
         <v/>
       </c>
@@ -3493,7 +3530,8 @@
       <c r="M123" s="23"/>
       <c r="N123" s="23"/>
     </row>
-    <row r="124" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="124" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A124" s="14"/>
       <c r="B124" s="6" t="str">
         <v/>
       </c>
@@ -3510,7 +3548,8 @@
       <c r="M124" s="23"/>
       <c r="N124" s="23"/>
     </row>
-    <row r="125" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="125" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A125" s="14"/>
       <c r="B125" s="6" t="str">
         <v/>
       </c>
@@ -3527,7 +3566,8 @@
       <c r="M125" s="23"/>
       <c r="N125" s="23"/>
     </row>
-    <row r="126" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="126" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A126" s="14"/>
       <c r="B126" s="6" t="str">
         <v/>
       </c>
@@ -3544,7 +3584,8 @@
       <c r="M126" s="23"/>
       <c r="N126" s="23"/>
     </row>
-    <row r="127" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="127" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A127" s="14"/>
       <c r="B127" s="6" t="str">
         <v/>
       </c>
@@ -3561,618 +3602,649 @@
       <c r="M127" s="23"/>
       <c r="N127" s="23"/>
     </row>
-    <row r="128" spans="2:14" s="14" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="130" spans="1:9" ht="25.5">
-      <c r="A130" s="25" t="s">
+    <row r="128" spans="1:14" ht="25.5">
+      <c r="A128" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B130" s="38"/>
-      <c r="C130" s="13" t="s">
+      <c r="B128" s="34"/>
+      <c r="C128" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D130" s="13" t="s">
+      <c r="D128" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E130" s="27"/>
-      <c r="F130" s="27"/>
-      <c r="G130" s="27"/>
-      <c r="H130" s="27"/>
+      <c r="E128" s="27"/>
+      <c r="F128" s="27"/>
+      <c r="G128" s="27"/>
+      <c r="H128" s="27"/>
+      <c r="I128" s="14"/>
+    </row>
+    <row r="129" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A129" s="28"/>
+      <c r="B129" s="26"/>
+      <c r="C129" s="45"/>
+      <c r="D129" s="45"/>
+      <c r="E129" s="45"/>
+      <c r="F129" s="45"/>
+      <c r="G129" s="45"/>
+      <c r="H129" s="45"/>
+      <c r="I129" s="14"/>
+    </row>
+    <row r="130" spans="1:9" ht="14.25" customHeight="1">
+      <c r="B130" s="26"/>
+      <c r="C130" s="45"/>
+      <c r="D130" s="45"/>
+      <c r="E130" s="45"/>
+      <c r="F130" s="45"/>
+      <c r="G130" s="45"/>
+      <c r="H130" s="45"/>
       <c r="I130" s="14"/>
     </row>
     <row r="131" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A131" s="28"/>
-      <c r="B131" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
-      <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
+      <c r="B131" s="26"/>
+      <c r="C131" s="45"/>
+      <c r="D131" s="45"/>
+      <c r="E131" s="45"/>
+      <c r="F131" s="45"/>
+      <c r="G131" s="45"/>
+      <c r="H131" s="45"/>
       <c r="I131" s="14"/>
     </row>
     <row r="132" spans="1:9" ht="14.25" customHeight="1">
-      <c r="B132" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
+      <c r="B132" s="26"/>
+      <c r="C132" s="45"/>
+      <c r="D132" s="45"/>
+      <c r="E132" s="45"/>
+      <c r="F132" s="45"/>
+      <c r="G132" s="45"/>
+      <c r="H132" s="45"/>
       <c r="I132" s="14"/>
     </row>
     <row r="133" spans="1:9" ht="14.25" customHeight="1">
-      <c r="B133" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
+      <c r="B133" s="26"/>
+      <c r="C133" s="46"/>
+      <c r="D133" s="46"/>
+      <c r="E133" s="46"/>
+      <c r="F133" s="46"/>
+      <c r="G133" s="46"/>
+      <c r="H133" s="46"/>
       <c r="I133" s="14"/>
     </row>
     <row r="134" spans="1:9" ht="14.25" customHeight="1">
-      <c r="B134" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2"/>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
+      <c r="B134" s="26"/>
+      <c r="C134" s="47"/>
+      <c r="D134" s="47"/>
+      <c r="E134" s="46"/>
+      <c r="F134" s="46"/>
+      <c r="G134" s="46"/>
+      <c r="H134" s="46"/>
       <c r="I134" s="14"/>
     </row>
     <row r="135" spans="1:9" ht="14.25" customHeight="1">
       <c r="B135" s="26"/>
-      <c r="C135" s="29"/>
-      <c r="D135" s="29"/>
-      <c r="E135" s="29"/>
-      <c r="F135" s="29"/>
-      <c r="G135" s="29"/>
-      <c r="H135" s="29"/>
+      <c r="C135" s="47"/>
+      <c r="D135" s="47"/>
+      <c r="E135" s="47"/>
+      <c r="F135" s="47"/>
+      <c r="G135" s="47"/>
+      <c r="H135" s="47"/>
       <c r="I135" s="14"/>
     </row>
     <row r="136" spans="1:9" ht="14.25" customHeight="1">
       <c r="B136" s="26"/>
-      <c r="C136" s="30"/>
-      <c r="D136" s="30"/>
-      <c r="E136" s="23"/>
-      <c r="F136" s="23"/>
-      <c r="G136" s="23"/>
-      <c r="H136" s="23"/>
+      <c r="C136" s="47"/>
+      <c r="D136" s="47"/>
+      <c r="E136" s="46"/>
+      <c r="F136" s="46"/>
+      <c r="G136" s="46"/>
+      <c r="H136" s="46"/>
       <c r="I136" s="14"/>
     </row>
     <row r="137" spans="1:9" ht="14.25" customHeight="1">
-      <c r="B137" s="26"/>
-      <c r="C137" s="30"/>
-      <c r="D137" s="30"/>
-      <c r="E137" s="30"/>
-      <c r="F137" s="30"/>
-      <c r="G137" s="30"/>
-      <c r="H137" s="30"/>
+      <c r="B137" s="42"/>
+      <c r="C137" s="48"/>
+      <c r="D137" s="48"/>
+      <c r="E137" s="48"/>
+      <c r="F137" s="48"/>
+      <c r="G137" s="48"/>
+      <c r="H137" s="48"/>
       <c r="I137" s="14"/>
     </row>
-    <row r="138" spans="1:9" ht="14.25" customHeight="1">
-      <c r="B138" s="26"/>
-      <c r="C138" s="30"/>
-      <c r="D138" s="30"/>
-      <c r="E138" s="23"/>
-      <c r="F138" s="23"/>
-      <c r="G138" s="23"/>
-      <c r="H138" s="23"/>
-      <c r="I138" s="14"/>
+    <row r="138" spans="1:9" ht="15.75">
+      <c r="A138" s="41"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="45"/>
+      <c r="D138" s="45"/>
+      <c r="E138" s="46"/>
+      <c r="F138" s="46"/>
+      <c r="G138" s="46"/>
+      <c r="H138" s="46"/>
     </row>
     <row r="139" spans="1:9" ht="14.25" customHeight="1">
-      <c r="B139" s="14"/>
-      <c r="C139" s="14"/>
-      <c r="D139" s="14"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="14"/>
-      <c r="H139" s="14"/>
-      <c r="I139" s="14"/>
-    </row>
-    <row r="140" spans="1:9" ht="15.75">
-      <c r="A140" s="25"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="45"/>
+      <c r="D139" s="45"/>
+      <c r="E139" s="46"/>
+      <c r="F139" s="46"/>
+      <c r="G139" s="46"/>
+      <c r="H139" s="46"/>
+    </row>
+    <row r="140" spans="1:9" ht="14.25" customHeight="1">
       <c r="B140" s="6"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
+      <c r="C140" s="45"/>
+      <c r="D140" s="45"/>
+      <c r="E140" s="46"/>
+      <c r="F140" s="46"/>
+      <c r="G140" s="46"/>
+      <c r="H140" s="46"/>
     </row>
     <row r="141" spans="1:9" ht="14.25" customHeight="1">
       <c r="B141" s="6"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
+      <c r="C141" s="45"/>
+      <c r="D141" s="45"/>
+      <c r="E141" s="46"/>
+      <c r="F141" s="46"/>
+      <c r="G141" s="46"/>
+      <c r="H141" s="46"/>
     </row>
     <row r="142" spans="1:9" ht="14.25" customHeight="1">
       <c r="B142" s="6"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
+      <c r="C142" s="45"/>
+      <c r="D142" s="45"/>
+      <c r="E142" s="46"/>
+      <c r="F142" s="46"/>
+      <c r="G142" s="46"/>
+      <c r="H142" s="46"/>
     </row>
     <row r="143" spans="1:9" ht="14.25" customHeight="1">
       <c r="B143" s="6"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
+      <c r="C143" s="45"/>
+      <c r="D143" s="45"/>
+      <c r="E143" s="46"/>
+      <c r="F143" s="46"/>
+      <c r="G143" s="46"/>
+      <c r="H143" s="46"/>
     </row>
     <row r="144" spans="1:9" ht="14.25" customHeight="1">
       <c r="B144" s="6"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
+      <c r="C144" s="45"/>
+      <c r="D144" s="45"/>
+      <c r="E144" s="46"/>
+      <c r="F144" s="46"/>
+      <c r="G144" s="46"/>
+      <c r="H144" s="46"/>
     </row>
     <row r="145" spans="1:14" ht="14.25" customHeight="1">
-      <c r="B145" s="32"/>
-      <c r="C145" s="33"/>
-      <c r="D145" s="33"/>
-    </row>
-    <row r="147" spans="1:14" ht="25.5">
-      <c r="A147" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B147" s="36"/>
-      <c r="C147" s="13" t="s">
+      <c r="B145" s="6"/>
+      <c r="C145" s="49"/>
+      <c r="D145" s="49"/>
+      <c r="E145" s="46"/>
+      <c r="F145" s="46"/>
+      <c r="G145" s="46"/>
+      <c r="H145" s="46"/>
+    </row>
+    <row r="146" spans="1:14" ht="14.25" customHeight="1">
+      <c r="B146" s="6"/>
+      <c r="C146" s="49"/>
+      <c r="D146" s="49"/>
+      <c r="E146" s="46"/>
+      <c r="F146" s="46"/>
+      <c r="G146" s="46"/>
+      <c r="H146" s="46"/>
+    </row>
+    <row r="147" spans="1:14" ht="14.25" customHeight="1">
+      <c r="B147" s="6"/>
+      <c r="C147" s="49"/>
+      <c r="D147" s="49"/>
+      <c r="E147" s="46"/>
+      <c r="F147" s="46"/>
+      <c r="G147" s="46"/>
+      <c r="H147" s="46"/>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="B148" s="44"/>
+      <c r="C148" s="46"/>
+      <c r="D148" s="46"/>
+      <c r="E148" s="46"/>
+      <c r="F148" s="46"/>
+      <c r="G148" s="46"/>
+      <c r="H148" s="46"/>
+    </row>
+    <row r="149" spans="1:14" ht="25.5">
+      <c r="A149" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B149" s="32"/>
+      <c r="C149" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D147" s="13" t="s">
+      <c r="D149" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E147" s="13" t="s">
+      <c r="E149" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F147" s="13" t="s">
+      <c r="F149" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G147" s="13" t="s">
+      <c r="G149" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H147" s="13" t="s">
+      <c r="H149" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I147" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J147" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="K147" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L147" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M147" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="N147" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14" ht="14.25" customHeight="1">
-      <c r="B148" s="6" t="str">
-        <f t="array" ref="B148:B167">IF(1*($AF$3:$AF$22="M")+($AF$3:$AF$22="C")*1,$B$3:$B$22,"")</f>
-        <v/>
-      </c>
-      <c r="C148" s="34"/>
-      <c r="D148" s="34"/>
-      <c r="E148" s="23"/>
-      <c r="F148" s="23"/>
-      <c r="G148" s="23"/>
-      <c r="H148" s="23"/>
-      <c r="I148" s="23"/>
-      <c r="J148" s="23"/>
-      <c r="K148" s="23"/>
-      <c r="L148" s="23"/>
-      <c r="M148" s="23"/>
-      <c r="N148" s="23"/>
-    </row>
-    <row r="149" spans="1:14" ht="14.25" customHeight="1">
-      <c r="B149" s="6" t="str">
-        <v/>
-      </c>
-      <c r="C149" s="34"/>
-      <c r="D149" s="34"/>
-      <c r="E149" s="23"/>
-      <c r="F149" s="23"/>
-      <c r="G149" s="23"/>
-      <c r="H149" s="23"/>
-      <c r="I149" s="23"/>
-      <c r="J149" s="23"/>
-      <c r="K149" s="23"/>
-      <c r="L149" s="23"/>
-      <c r="M149" s="23"/>
-      <c r="N149" s="23"/>
+      <c r="I149" s="50"/>
+      <c r="J149" s="50"/>
+      <c r="K149" s="50"/>
+      <c r="L149" s="50"/>
+      <c r="M149" s="50"/>
+      <c r="N149" s="50"/>
     </row>
     <row r="150" spans="1:14" ht="14.25" customHeight="1">
       <c r="B150" s="6" t="str">
-        <v/>
-      </c>
-      <c r="C150" s="34"/>
-      <c r="D150" s="34"/>
-      <c r="E150" s="23"/>
-      <c r="F150" s="23"/>
-      <c r="G150" s="23"/>
-      <c r="H150" s="23"/>
-      <c r="I150" s="23"/>
-      <c r="J150" s="23"/>
-      <c r="K150" s="23"/>
-      <c r="L150" s="23"/>
-      <c r="M150" s="23"/>
-      <c r="N150" s="23"/>
+        <f t="array" ref="B150:B169">IF(1*($AF$3:$AF$22="M")+($AF$3:$AF$22="C")*1,$B$3:$B$22,"")</f>
+        <v/>
+      </c>
+      <c r="C150" s="46"/>
+      <c r="D150" s="46"/>
+      <c r="E150" s="46"/>
+      <c r="F150" s="46"/>
+      <c r="G150" s="46"/>
+      <c r="H150" s="46"/>
+      <c r="I150" s="51"/>
+      <c r="J150" s="51"/>
+      <c r="K150" s="51"/>
+      <c r="L150" s="51"/>
+      <c r="M150" s="51"/>
+      <c r="N150" s="51"/>
     </row>
     <row r="151" spans="1:14" ht="14.25" customHeight="1">
       <c r="B151" s="6" t="str">
         <v/>
       </c>
-      <c r="C151" s="34"/>
-      <c r="D151" s="34"/>
-      <c r="E151" s="23"/>
-      <c r="F151" s="23"/>
-      <c r="G151" s="23"/>
-      <c r="H151" s="23"/>
-      <c r="I151" s="23"/>
-      <c r="J151" s="23"/>
-      <c r="K151" s="23"/>
-      <c r="L151" s="23"/>
-      <c r="M151" s="23"/>
-      <c r="N151" s="23"/>
+      <c r="C151" s="46"/>
+      <c r="D151" s="46"/>
+      <c r="E151" s="46"/>
+      <c r="F151" s="46"/>
+      <c r="G151" s="46"/>
+      <c r="H151" s="46"/>
+      <c r="I151" s="51"/>
+      <c r="J151" s="51"/>
+      <c r="K151" s="51"/>
+      <c r="L151" s="51"/>
+      <c r="M151" s="51"/>
+      <c r="N151" s="51"/>
     </row>
     <row r="152" spans="1:14" ht="14.25" customHeight="1">
       <c r="B152" s="6" t="str">
         <v/>
       </c>
-      <c r="C152" s="34"/>
-      <c r="D152" s="34"/>
-      <c r="E152" s="23"/>
-      <c r="F152" s="23"/>
-      <c r="G152" s="23"/>
-      <c r="H152" s="23"/>
-      <c r="I152" s="23"/>
-      <c r="J152" s="23"/>
-      <c r="K152" s="23"/>
-      <c r="L152" s="23"/>
-      <c r="M152" s="23"/>
-      <c r="N152" s="23"/>
+      <c r="C152" s="46"/>
+      <c r="D152" s="46"/>
+      <c r="E152" s="46"/>
+      <c r="F152" s="46"/>
+      <c r="G152" s="46"/>
+      <c r="H152" s="46"/>
+      <c r="I152" s="51"/>
+      <c r="J152" s="51"/>
+      <c r="K152" s="51"/>
+      <c r="L152" s="51"/>
+      <c r="M152" s="51"/>
+      <c r="N152" s="51"/>
     </row>
     <row r="153" spans="1:14" ht="14.25" customHeight="1">
-      <c r="A153" s="14"/>
       <c r="B153" s="6" t="str">
         <v/>
       </c>
-      <c r="C153" s="34"/>
-      <c r="D153" s="34"/>
-      <c r="E153" s="23"/>
-      <c r="F153" s="23"/>
-      <c r="G153" s="23"/>
-      <c r="H153" s="23"/>
-      <c r="I153" s="23"/>
-      <c r="J153" s="23"/>
-      <c r="K153" s="23"/>
-      <c r="L153" s="23"/>
-      <c r="M153" s="23"/>
-      <c r="N153" s="23"/>
+      <c r="C153" s="46"/>
+      <c r="D153" s="46"/>
+      <c r="E153" s="46"/>
+      <c r="F153" s="46"/>
+      <c r="G153" s="46"/>
+      <c r="H153" s="46"/>
+      <c r="I153" s="51"/>
+      <c r="J153" s="51"/>
+      <c r="K153" s="51"/>
+      <c r="L153" s="51"/>
+      <c r="M153" s="51"/>
+      <c r="N153" s="51"/>
     </row>
     <row r="154" spans="1:14" ht="14.25" customHeight="1">
-      <c r="A154" s="14"/>
       <c r="B154" s="6" t="str">
         <v/>
       </c>
-      <c r="C154" s="34"/>
-      <c r="D154" s="34"/>
-      <c r="E154" s="23"/>
-      <c r="F154" s="23"/>
-      <c r="G154" s="23"/>
-      <c r="H154" s="23"/>
-      <c r="I154" s="23"/>
-      <c r="J154" s="23"/>
-      <c r="K154" s="23"/>
-      <c r="L154" s="23"/>
-      <c r="M154" s="23"/>
-      <c r="N154" s="23"/>
+      <c r="C154" s="46"/>
+      <c r="D154" s="46"/>
+      <c r="E154" s="46"/>
+      <c r="F154" s="46"/>
+      <c r="G154" s="46"/>
+      <c r="H154" s="46"/>
+      <c r="I154" s="51"/>
+      <c r="J154" s="51"/>
+      <c r="K154" s="51"/>
+      <c r="L154" s="51"/>
+      <c r="M154" s="51"/>
+      <c r="N154" s="51"/>
     </row>
     <row r="155" spans="1:14" ht="14.25" customHeight="1">
       <c r="A155" s="14"/>
       <c r="B155" s="6" t="str">
         <v/>
       </c>
-      <c r="C155" s="34"/>
-      <c r="D155" s="34"/>
-      <c r="E155" s="23"/>
-      <c r="F155" s="23"/>
-      <c r="G155" s="23"/>
-      <c r="H155" s="23"/>
-      <c r="I155" s="23"/>
-      <c r="J155" s="23"/>
-      <c r="K155" s="23"/>
-      <c r="L155" s="23"/>
-      <c r="M155" s="23"/>
-      <c r="N155" s="23"/>
+      <c r="C155" s="46"/>
+      <c r="D155" s="46"/>
+      <c r="E155" s="46"/>
+      <c r="F155" s="46"/>
+      <c r="G155" s="46"/>
+      <c r="H155" s="46"/>
+      <c r="I155" s="51"/>
+      <c r="J155" s="51"/>
+      <c r="K155" s="51"/>
+      <c r="L155" s="51"/>
+      <c r="M155" s="51"/>
+      <c r="N155" s="51"/>
     </row>
     <row r="156" spans="1:14" ht="14.25" customHeight="1">
       <c r="A156" s="14"/>
       <c r="B156" s="6" t="str">
         <v/>
       </c>
-      <c r="C156" s="34"/>
-      <c r="D156" s="34"/>
-      <c r="E156" s="23"/>
-      <c r="F156" s="23"/>
-      <c r="G156" s="23"/>
-      <c r="H156" s="23"/>
-      <c r="I156" s="23"/>
-      <c r="J156" s="23"/>
-      <c r="K156" s="23"/>
-      <c r="L156" s="23"/>
-      <c r="M156" s="23"/>
-      <c r="N156" s="23"/>
+      <c r="C156" s="46"/>
+      <c r="D156" s="46"/>
+      <c r="E156" s="46"/>
+      <c r="F156" s="46"/>
+      <c r="G156" s="46"/>
+      <c r="H156" s="46"/>
+      <c r="I156" s="51"/>
+      <c r="J156" s="51"/>
+      <c r="K156" s="51"/>
+      <c r="L156" s="51"/>
+      <c r="M156" s="51"/>
+      <c r="N156" s="51"/>
     </row>
     <row r="157" spans="1:14" ht="14.25" customHeight="1">
       <c r="A157" s="14"/>
       <c r="B157" s="6" t="str">
         <v/>
       </c>
-      <c r="C157" s="34"/>
-      <c r="D157" s="34"/>
-      <c r="E157" s="23"/>
-      <c r="F157" s="23"/>
-      <c r="G157" s="23"/>
-      <c r="H157" s="23"/>
-      <c r="I157" s="23"/>
-      <c r="J157" s="23"/>
-      <c r="K157" s="23"/>
-      <c r="L157" s="23"/>
-      <c r="M157" s="23"/>
-      <c r="N157" s="23"/>
+      <c r="C157" s="46"/>
+      <c r="D157" s="46"/>
+      <c r="E157" s="46"/>
+      <c r="F157" s="46"/>
+      <c r="G157" s="46"/>
+      <c r="H157" s="46"/>
+      <c r="I157" s="51"/>
+      <c r="J157" s="51"/>
+      <c r="K157" s="51"/>
+      <c r="L157" s="51"/>
+      <c r="M157" s="51"/>
+      <c r="N157" s="51"/>
     </row>
     <row r="158" spans="1:14" ht="14.25" customHeight="1">
       <c r="A158" s="14"/>
       <c r="B158" s="6" t="str">
         <v/>
       </c>
-      <c r="C158" s="34"/>
-      <c r="D158" s="34"/>
-      <c r="E158" s="23"/>
-      <c r="F158" s="23"/>
-      <c r="G158" s="23"/>
-      <c r="H158" s="23"/>
-      <c r="I158" s="23"/>
-      <c r="J158" s="23"/>
-      <c r="K158" s="23"/>
-      <c r="L158" s="23"/>
-      <c r="M158" s="23"/>
-      <c r="N158" s="23"/>
+      <c r="C158" s="46"/>
+      <c r="D158" s="46"/>
+      <c r="E158" s="46"/>
+      <c r="F158" s="46"/>
+      <c r="G158" s="46"/>
+      <c r="H158" s="46"/>
+      <c r="I158" s="51"/>
+      <c r="J158" s="51"/>
+      <c r="K158" s="51"/>
+      <c r="L158" s="51"/>
+      <c r="M158" s="51"/>
+      <c r="N158" s="51"/>
     </row>
     <row r="159" spans="1:14" ht="14.25" customHeight="1">
       <c r="A159" s="14"/>
       <c r="B159" s="6" t="str">
         <v/>
       </c>
-      <c r="C159" s="34"/>
-      <c r="D159" s="34"/>
-      <c r="E159" s="23"/>
-      <c r="F159" s="23"/>
-      <c r="G159" s="23"/>
-      <c r="H159" s="23"/>
-      <c r="I159" s="23"/>
-      <c r="J159" s="23"/>
-      <c r="K159" s="23"/>
-      <c r="L159" s="23"/>
-      <c r="M159" s="23"/>
-      <c r="N159" s="23"/>
+      <c r="C159" s="46"/>
+      <c r="D159" s="46"/>
+      <c r="E159" s="46"/>
+      <c r="F159" s="46"/>
+      <c r="G159" s="46"/>
+      <c r="H159" s="46"/>
+      <c r="I159" s="51"/>
+      <c r="J159" s="51"/>
+      <c r="K159" s="51"/>
+      <c r="L159" s="51"/>
+      <c r="M159" s="51"/>
+      <c r="N159" s="51"/>
     </row>
     <row r="160" spans="1:14" ht="14.25" customHeight="1">
       <c r="A160" s="14"/>
       <c r="B160" s="6" t="str">
         <v/>
       </c>
-      <c r="C160" s="34"/>
-      <c r="D160" s="34"/>
-      <c r="E160" s="23"/>
-      <c r="F160" s="23"/>
-      <c r="G160" s="23"/>
-      <c r="H160" s="23"/>
-      <c r="I160" s="23"/>
-      <c r="J160" s="23"/>
-      <c r="K160" s="23"/>
-      <c r="L160" s="23"/>
-      <c r="M160" s="23"/>
-      <c r="N160" s="23"/>
+      <c r="C160" s="46"/>
+      <c r="D160" s="46"/>
+      <c r="E160" s="46"/>
+      <c r="F160" s="46"/>
+      <c r="G160" s="46"/>
+      <c r="H160" s="46"/>
+      <c r="I160" s="51"/>
+      <c r="J160" s="51"/>
+      <c r="K160" s="51"/>
+      <c r="L160" s="51"/>
+      <c r="M160" s="51"/>
+      <c r="N160" s="51"/>
     </row>
     <row r="161" spans="1:14" ht="14.25" customHeight="1">
       <c r="A161" s="14"/>
       <c r="B161" s="6" t="str">
         <v/>
       </c>
-      <c r="C161" s="34"/>
-      <c r="D161" s="34"/>
-      <c r="E161" s="23"/>
-      <c r="F161" s="23"/>
-      <c r="G161" s="23"/>
-      <c r="H161" s="23"/>
-      <c r="I161" s="23"/>
-      <c r="J161" s="23"/>
-      <c r="K161" s="23"/>
-      <c r="L161" s="23"/>
-      <c r="M161" s="23"/>
-      <c r="N161" s="23"/>
+      <c r="C161" s="46"/>
+      <c r="D161" s="46"/>
+      <c r="E161" s="46"/>
+      <c r="F161" s="46"/>
+      <c r="G161" s="46"/>
+      <c r="H161" s="46"/>
+      <c r="I161" s="51"/>
+      <c r="J161" s="51"/>
+      <c r="K161" s="51"/>
+      <c r="L161" s="51"/>
+      <c r="M161" s="51"/>
+      <c r="N161" s="51"/>
     </row>
     <row r="162" spans="1:14" ht="14.25" customHeight="1">
       <c r="A162" s="14"/>
-      <c r="B162" s="24" t="str">
-        <v/>
-      </c>
-      <c r="C162" s="34"/>
-      <c r="D162" s="34"/>
-      <c r="E162" s="23"/>
-      <c r="F162" s="23"/>
-      <c r="G162" s="23"/>
-      <c r="H162" s="23"/>
-      <c r="I162" s="23"/>
-      <c r="J162" s="23"/>
-      <c r="K162" s="23"/>
-      <c r="L162" s="23"/>
-      <c r="M162" s="23"/>
-      <c r="N162" s="23"/>
+      <c r="B162" s="6" t="str">
+        <v/>
+      </c>
+      <c r="C162" s="46"/>
+      <c r="D162" s="46"/>
+      <c r="E162" s="46"/>
+      <c r="F162" s="46"/>
+      <c r="G162" s="46"/>
+      <c r="H162" s="46"/>
+      <c r="I162" s="51"/>
+      <c r="J162" s="51"/>
+      <c r="K162" s="51"/>
+      <c r="L162" s="51"/>
+      <c r="M162" s="51"/>
+      <c r="N162" s="51"/>
     </row>
     <row r="163" spans="1:14" ht="14.25" customHeight="1">
       <c r="A163" s="14"/>
       <c r="B163" s="6" t="str">
         <v/>
       </c>
-      <c r="C163" s="34"/>
-      <c r="D163" s="34"/>
-      <c r="E163" s="23"/>
-      <c r="F163" s="23"/>
-      <c r="G163" s="23"/>
-      <c r="H163" s="23"/>
-      <c r="I163" s="23"/>
-      <c r="J163" s="23"/>
-      <c r="K163" s="23"/>
-      <c r="L163" s="23"/>
-      <c r="M163" s="23"/>
-      <c r="N163" s="23"/>
+      <c r="C163" s="46"/>
+      <c r="D163" s="46"/>
+      <c r="E163" s="46"/>
+      <c r="F163" s="46"/>
+      <c r="G163" s="46"/>
+      <c r="H163" s="46"/>
+      <c r="I163" s="51"/>
+      <c r="J163" s="51"/>
+      <c r="K163" s="51"/>
+      <c r="L163" s="51"/>
+      <c r="M163" s="51"/>
+      <c r="N163" s="51"/>
     </row>
     <row r="164" spans="1:14" ht="14.25" customHeight="1">
       <c r="A164" s="14"/>
-      <c r="B164" s="6" t="str">
-        <v/>
-      </c>
-      <c r="C164" s="34"/>
-      <c r="D164" s="34"/>
-      <c r="E164" s="23"/>
-      <c r="F164" s="23"/>
-      <c r="G164" s="23"/>
-      <c r="H164" s="23"/>
-      <c r="I164" s="23"/>
-      <c r="J164" s="23"/>
-      <c r="K164" s="23"/>
-      <c r="L164" s="23"/>
-      <c r="M164" s="23"/>
-      <c r="N164" s="23"/>
+      <c r="B164" s="24" t="str">
+        <v/>
+      </c>
+      <c r="C164" s="46"/>
+      <c r="D164" s="46"/>
+      <c r="E164" s="46"/>
+      <c r="F164" s="46"/>
+      <c r="G164" s="46"/>
+      <c r="H164" s="46"/>
+      <c r="I164" s="51"/>
+      <c r="J164" s="51"/>
+      <c r="K164" s="51"/>
+      <c r="L164" s="51"/>
+      <c r="M164" s="51"/>
+      <c r="N164" s="51"/>
     </row>
     <row r="165" spans="1:14" ht="14.25" customHeight="1">
       <c r="A165" s="14"/>
       <c r="B165" s="6" t="str">
         <v/>
       </c>
-      <c r="C165" s="34"/>
-      <c r="D165" s="34"/>
-      <c r="E165" s="23"/>
-      <c r="F165" s="23"/>
-      <c r="G165" s="23"/>
-      <c r="H165" s="23"/>
-      <c r="I165" s="23"/>
-      <c r="J165" s="23"/>
-      <c r="K165" s="23"/>
-      <c r="L165" s="23"/>
-      <c r="M165" s="23"/>
-      <c r="N165" s="23"/>
+      <c r="C165" s="46"/>
+      <c r="D165" s="46"/>
+      <c r="E165" s="46"/>
+      <c r="F165" s="46"/>
+      <c r="G165" s="46"/>
+      <c r="H165" s="46"/>
+      <c r="I165" s="51"/>
+      <c r="J165" s="51"/>
+      <c r="K165" s="51"/>
+      <c r="L165" s="51"/>
+      <c r="M165" s="51"/>
+      <c r="N165" s="51"/>
     </row>
     <row r="166" spans="1:14" ht="14.25" customHeight="1">
       <c r="A166" s="14"/>
       <c r="B166" s="6" t="str">
         <v/>
       </c>
-      <c r="C166" s="34"/>
-      <c r="D166" s="34"/>
-      <c r="E166" s="23"/>
-      <c r="F166" s="23"/>
-      <c r="G166" s="23"/>
-      <c r="H166" s="23"/>
-      <c r="I166" s="23"/>
-      <c r="J166" s="23"/>
-      <c r="K166" s="23"/>
-      <c r="L166" s="23"/>
-      <c r="M166" s="23"/>
-      <c r="N166" s="23"/>
+      <c r="C166" s="46"/>
+      <c r="D166" s="46"/>
+      <c r="E166" s="46"/>
+      <c r="F166" s="46"/>
+      <c r="G166" s="46"/>
+      <c r="H166" s="46"/>
+      <c r="I166" s="51"/>
+      <c r="J166" s="51"/>
+      <c r="K166" s="51"/>
+      <c r="L166" s="51"/>
+      <c r="M166" s="51"/>
+      <c r="N166" s="51"/>
     </row>
     <row r="167" spans="1:14" ht="14.25" customHeight="1">
       <c r="A167" s="14"/>
       <c r="B167" s="6" t="str">
         <v/>
       </c>
-      <c r="C167" s="34"/>
-      <c r="D167" s="34"/>
-      <c r="E167" s="23"/>
-      <c r="F167" s="23"/>
-      <c r="G167" s="23"/>
-      <c r="H167" s="23"/>
-      <c r="I167" s="23"/>
-      <c r="J167" s="23"/>
-      <c r="K167" s="23"/>
-      <c r="L167" s="23"/>
-      <c r="M167" s="23"/>
-      <c r="N167" s="23"/>
-    </row>
-    <row r="169" spans="1:14" ht="25.5">
-      <c r="A169" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B169" s="36"/>
-      <c r="C169" s="13" t="s">
+      <c r="C167" s="46"/>
+      <c r="D167" s="46"/>
+      <c r="E167" s="46"/>
+      <c r="F167" s="46"/>
+      <c r="G167" s="46"/>
+      <c r="H167" s="46"/>
+      <c r="I167" s="51"/>
+      <c r="J167" s="51"/>
+      <c r="K167" s="51"/>
+      <c r="L167" s="51"/>
+      <c r="M167" s="51"/>
+      <c r="N167" s="51"/>
+    </row>
+    <row r="168" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A168" s="14"/>
+      <c r="B168" s="6" t="str">
+        <v/>
+      </c>
+      <c r="C168" s="46"/>
+      <c r="D168" s="46"/>
+      <c r="E168" s="46"/>
+      <c r="F168" s="46"/>
+      <c r="G168" s="46"/>
+      <c r="H168" s="46"/>
+      <c r="I168" s="51"/>
+      <c r="J168" s="51"/>
+      <c r="K168" s="51"/>
+      <c r="L168" s="51"/>
+      <c r="M168" s="51"/>
+      <c r="N168" s="51"/>
+    </row>
+    <row r="169" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A169" s="14"/>
+      <c r="B169" s="6" t="str">
+        <v/>
+      </c>
+      <c r="C169" s="46"/>
+      <c r="D169" s="46"/>
+      <c r="E169" s="46"/>
+      <c r="F169" s="46"/>
+      <c r="G169" s="46"/>
+      <c r="H169" s="46"/>
+      <c r="I169" s="51"/>
+      <c r="J169" s="51"/>
+      <c r="K169" s="51"/>
+      <c r="L169" s="51"/>
+      <c r="M169" s="51"/>
+      <c r="N169" s="51"/>
+    </row>
+    <row r="170" spans="1:14" ht="25.5">
+      <c r="A170" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B170" s="32"/>
+      <c r="C170" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D169" s="13" t="s">
+      <c r="D170" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E169" s="13" t="s">
+      <c r="E170" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F169" s="13" t="s">
+      <c r="F170" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G169" s="13" t="s">
+      <c r="G170" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H169" s="13" t="s">
+      <c r="H170" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I169" s="13" t="s">
+      <c r="I170" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J169" s="13" t="s">
+      <c r="J170" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="K169" s="13" t="s">
+      <c r="K170" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="L169" s="13" t="s">
+      <c r="L170" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="M169" s="13" t="s">
+      <c r="M170" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N169" s="13" t="s">
+      <c r="N170" s="13" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="170" spans="1:14" ht="14.25" customHeight="1">
-      <c r="B170" s="6" t="str">
-        <f t="array" ref="B170:B189">IF(1*($AG$3:$AG$22="M")+($AG$3:$AG$22="C")*1,$B$3:$B$22,"")</f>
-        <v/>
-      </c>
-      <c r="C170" s="34"/>
-      <c r="D170" s="34"/>
-      <c r="E170" s="23"/>
-      <c r="F170" s="23"/>
-      <c r="G170" s="23"/>
-      <c r="H170" s="23"/>
-      <c r="I170" s="23"/>
-      <c r="J170" s="23"/>
-      <c r="K170" s="23"/>
-      <c r="L170" s="23"/>
-      <c r="M170" s="23"/>
-      <c r="N170" s="23"/>
     </row>
     <row r="171" spans="1:14" ht="14.25" customHeight="1">
       <c r="B171" s="6" t="str">
-        <v/>
-      </c>
-      <c r="C171" s="34"/>
-      <c r="D171" s="34"/>
+        <f t="array" ref="B171:B190">IF(1*($AG$3:$AG$22="M")+($AG$3:$AG$22="C")*1,$B$3:$B$22,"")</f>
+        <v/>
+      </c>
+      <c r="C171" s="30"/>
+      <c r="D171" s="30"/>
       <c r="E171" s="23"/>
       <c r="F171" s="23"/>
       <c r="G171" s="23"/>
@@ -4188,8 +4260,8 @@
       <c r="B172" s="6" t="str">
         <v/>
       </c>
-      <c r="C172" s="34"/>
-      <c r="D172" s="34"/>
+      <c r="C172" s="30"/>
+      <c r="D172" s="30"/>
       <c r="E172" s="23"/>
       <c r="F172" s="23"/>
       <c r="G172" s="23"/>
@@ -4205,8 +4277,8 @@
       <c r="B173" s="6" t="str">
         <v/>
       </c>
-      <c r="C173" s="34"/>
-      <c r="D173" s="34"/>
+      <c r="C173" s="30"/>
+      <c r="D173" s="30"/>
       <c r="E173" s="23"/>
       <c r="F173" s="23"/>
       <c r="G173" s="23"/>
@@ -4222,8 +4294,8 @@
       <c r="B174" s="6" t="str">
         <v/>
       </c>
-      <c r="C174" s="34"/>
-      <c r="D174" s="34"/>
+      <c r="C174" s="30"/>
+      <c r="D174" s="30"/>
       <c r="E174" s="23"/>
       <c r="F174" s="23"/>
       <c r="G174" s="23"/>
@@ -4236,12 +4308,11 @@
       <c r="N174" s="23"/>
     </row>
     <row r="175" spans="1:14" ht="14.25" customHeight="1">
-      <c r="A175" s="14"/>
       <c r="B175" s="6" t="str">
         <v/>
       </c>
-      <c r="C175" s="34"/>
-      <c r="D175" s="34"/>
+      <c r="C175" s="30"/>
+      <c r="D175" s="30"/>
       <c r="E175" s="23"/>
       <c r="F175" s="23"/>
       <c r="G175" s="23"/>
@@ -4258,8 +4329,8 @@
       <c r="B176" s="6" t="str">
         <v/>
       </c>
-      <c r="C176" s="34"/>
-      <c r="D176" s="34"/>
+      <c r="C176" s="30"/>
+      <c r="D176" s="30"/>
       <c r="E176" s="23"/>
       <c r="F176" s="23"/>
       <c r="G176" s="23"/>
@@ -4276,8 +4347,8 @@
       <c r="B177" s="6" t="str">
         <v/>
       </c>
-      <c r="C177" s="34"/>
-      <c r="D177" s="34"/>
+      <c r="C177" s="30"/>
+      <c r="D177" s="30"/>
       <c r="E177" s="23"/>
       <c r="F177" s="23"/>
       <c r="G177" s="23"/>
@@ -4294,8 +4365,8 @@
       <c r="B178" s="6" t="str">
         <v/>
       </c>
-      <c r="C178" s="34"/>
-      <c r="D178" s="34"/>
+      <c r="C178" s="30"/>
+      <c r="D178" s="30"/>
       <c r="E178" s="23"/>
       <c r="F178" s="23"/>
       <c r="G178" s="23"/>
@@ -4312,8 +4383,8 @@
       <c r="B179" s="6" t="str">
         <v/>
       </c>
-      <c r="C179" s="34"/>
-      <c r="D179" s="34"/>
+      <c r="C179" s="30"/>
+      <c r="D179" s="30"/>
       <c r="E179" s="23"/>
       <c r="F179" s="23"/>
       <c r="G179" s="23"/>
@@ -4330,8 +4401,8 @@
       <c r="B180" s="6" t="str">
         <v/>
       </c>
-      <c r="C180" s="34"/>
-      <c r="D180" s="34"/>
+      <c r="C180" s="30"/>
+      <c r="D180" s="30"/>
       <c r="E180" s="23"/>
       <c r="F180" s="23"/>
       <c r="G180" s="23"/>
@@ -4348,8 +4419,8 @@
       <c r="B181" s="6" t="str">
         <v/>
       </c>
-      <c r="C181" s="34"/>
-      <c r="D181" s="34"/>
+      <c r="C181" s="30"/>
+      <c r="D181" s="30"/>
       <c r="E181" s="23"/>
       <c r="F181" s="23"/>
       <c r="G181" s="23"/>
@@ -4366,8 +4437,8 @@
       <c r="B182" s="6" t="str">
         <v/>
       </c>
-      <c r="C182" s="34"/>
-      <c r="D182" s="34"/>
+      <c r="C182" s="30"/>
+      <c r="D182" s="30"/>
       <c r="E182" s="23"/>
       <c r="F182" s="23"/>
       <c r="G182" s="23"/>
@@ -4384,8 +4455,8 @@
       <c r="B183" s="6" t="str">
         <v/>
       </c>
-      <c r="C183" s="34"/>
-      <c r="D183" s="34"/>
+      <c r="C183" s="30"/>
+      <c r="D183" s="30"/>
       <c r="E183" s="23"/>
       <c r="F183" s="23"/>
       <c r="G183" s="23"/>
@@ -4399,11 +4470,11 @@
     </row>
     <row r="184" spans="1:14" ht="14.25" customHeight="1">
       <c r="A184" s="14"/>
-      <c r="B184" s="24" t="str">
-        <v/>
-      </c>
-      <c r="C184" s="34"/>
-      <c r="D184" s="34"/>
+      <c r="B184" s="6" t="str">
+        <v/>
+      </c>
+      <c r="C184" s="30"/>
+      <c r="D184" s="30"/>
       <c r="E184" s="23"/>
       <c r="F184" s="23"/>
       <c r="G184" s="23"/>
@@ -4417,11 +4488,11 @@
     </row>
     <row r="185" spans="1:14" ht="14.25" customHeight="1">
       <c r="A185" s="14"/>
-      <c r="B185" s="6" t="str">
-        <v/>
-      </c>
-      <c r="C185" s="34"/>
-      <c r="D185" s="34"/>
+      <c r="B185" s="24" t="str">
+        <v/>
+      </c>
+      <c r="C185" s="30"/>
+      <c r="D185" s="30"/>
       <c r="E185" s="23"/>
       <c r="F185" s="23"/>
       <c r="G185" s="23"/>
@@ -4438,8 +4509,8 @@
       <c r="B186" s="6" t="str">
         <v/>
       </c>
-      <c r="C186" s="34"/>
-      <c r="D186" s="34"/>
+      <c r="C186" s="30"/>
+      <c r="D186" s="30"/>
       <c r="E186" s="23"/>
       <c r="F186" s="23"/>
       <c r="G186" s="23"/>
@@ -4456,8 +4527,8 @@
       <c r="B187" s="6" t="str">
         <v/>
       </c>
-      <c r="C187" s="34"/>
-      <c r="D187" s="34"/>
+      <c r="C187" s="30"/>
+      <c r="D187" s="30"/>
       <c r="E187" s="23"/>
       <c r="F187" s="23"/>
       <c r="G187" s="23"/>
@@ -4474,8 +4545,8 @@
       <c r="B188" s="6" t="str">
         <v/>
       </c>
-      <c r="C188" s="34"/>
-      <c r="D188" s="34"/>
+      <c r="C188" s="30"/>
+      <c r="D188" s="30"/>
       <c r="E188" s="23"/>
       <c r="F188" s="23"/>
       <c r="G188" s="23"/>
@@ -4492,8 +4563,8 @@
       <c r="B189" s="6" t="str">
         <v/>
       </c>
-      <c r="C189" s="34"/>
-      <c r="D189" s="34"/>
+      <c r="C189" s="30"/>
+      <c r="D189" s="30"/>
       <c r="E189" s="23"/>
       <c r="F189" s="23"/>
       <c r="G189" s="23"/>
@@ -4505,69 +4576,498 @@
       <c r="M189" s="23"/>
       <c r="N189" s="23"/>
     </row>
-    <row r="206" spans="3:10">
-      <c r="C206" s="40"/>
-      <c r="D206" s="40"/>
-      <c r="E206" s="40"/>
-      <c r="F206" s="40"/>
-      <c r="G206" s="40"/>
-      <c r="H206" s="40"/>
-      <c r="I206" s="41"/>
-      <c r="J206" s="40"/>
-    </row>
-    <row r="207" spans="3:10">
-      <c r="J207" s="39"/>
-    </row>
-    <row r="208" spans="3:10">
-      <c r="J208" s="39"/>
-    </row>
-    <row r="209" spans="3:10">
-      <c r="J209" s="39"/>
-    </row>
-    <row r="210" spans="3:10">
-      <c r="J210" s="39"/>
-    </row>
-    <row r="211" spans="3:10">
-      <c r="J211" s="39"/>
-    </row>
-    <row r="222" spans="3:10">
-      <c r="C222" s="40"/>
-    </row>
-    <row r="240" spans="3:7">
-      <c r="C240" s="41"/>
-      <c r="D240" s="41"/>
-      <c r="E240" s="41"/>
-      <c r="F240" s="41"/>
-      <c r="G240" s="41"/>
+    <row r="190" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A190" s="14"/>
+      <c r="B190" s="24" t="str">
+        <v/>
+      </c>
+      <c r="C190" s="53"/>
+      <c r="D190" s="53"/>
+      <c r="E190" s="54"/>
+      <c r="F190" s="54"/>
+      <c r="G190" s="54"/>
+      <c r="H190" s="54"/>
+      <c r="I190" s="54"/>
+      <c r="J190" s="54"/>
+      <c r="K190" s="54"/>
+      <c r="L190" s="54"/>
+      <c r="M190" s="54"/>
+      <c r="N190" s="54"/>
+    </row>
+    <row r="191" spans="1:14">
+      <c r="A191" s="5"/>
+      <c r="B191" s="62"/>
+      <c r="C191" s="55"/>
+      <c r="D191" s="55"/>
+      <c r="E191" s="55"/>
+      <c r="F191" s="55"/>
+      <c r="G191" s="55"/>
+      <c r="H191" s="55"/>
+      <c r="I191" s="55"/>
+      <c r="J191" s="63"/>
+      <c r="K191" s="63"/>
+      <c r="L191" s="63"/>
+      <c r="M191" s="63"/>
+      <c r="N191" s="63"/>
+    </row>
+    <row r="192" spans="1:14">
+      <c r="B192" s="44"/>
+      <c r="C192" s="52"/>
+      <c r="D192" s="52"/>
+      <c r="E192" s="57"/>
+      <c r="F192" s="57"/>
+      <c r="G192" s="57"/>
+      <c r="H192" s="57"/>
+      <c r="I192" s="57"/>
+      <c r="J192" s="58"/>
+      <c r="K192" s="58"/>
+      <c r="L192" s="58"/>
+      <c r="M192" s="58"/>
+      <c r="N192" s="58"/>
+    </row>
+    <row r="193" spans="2:14">
+      <c r="B193" s="44"/>
+      <c r="C193" s="52"/>
+      <c r="D193" s="52"/>
+      <c r="E193" s="57"/>
+      <c r="F193" s="57"/>
+      <c r="G193" s="57"/>
+      <c r="H193" s="57"/>
+      <c r="I193" s="57"/>
+      <c r="J193" s="58"/>
+      <c r="K193" s="58"/>
+      <c r="L193" s="58"/>
+      <c r="M193" s="58"/>
+      <c r="N193" s="58"/>
+    </row>
+    <row r="194" spans="2:14">
+      <c r="B194" s="44"/>
+      <c r="C194" s="52"/>
+      <c r="D194" s="52"/>
+      <c r="E194" s="57"/>
+      <c r="F194" s="57"/>
+      <c r="G194" s="57"/>
+      <c r="H194" s="57"/>
+      <c r="I194" s="57"/>
+      <c r="J194" s="58"/>
+      <c r="K194" s="58"/>
+      <c r="L194" s="58"/>
+      <c r="M194" s="58"/>
+      <c r="N194" s="58"/>
+    </row>
+    <row r="195" spans="2:14">
+      <c r="B195" s="44"/>
+      <c r="C195" s="52"/>
+      <c r="D195" s="52"/>
+      <c r="E195" s="57"/>
+      <c r="F195" s="57"/>
+      <c r="G195" s="57"/>
+      <c r="H195" s="57"/>
+      <c r="I195" s="57"/>
+      <c r="J195" s="58"/>
+      <c r="K195" s="58"/>
+      <c r="L195" s="58"/>
+      <c r="M195" s="58"/>
+      <c r="N195" s="58"/>
+    </row>
+    <row r="196" spans="2:14">
+      <c r="B196" s="44"/>
+      <c r="C196" s="52"/>
+      <c r="D196" s="52"/>
+      <c r="E196" s="57"/>
+      <c r="F196" s="57"/>
+      <c r="G196" s="57"/>
+      <c r="H196" s="57"/>
+      <c r="I196" s="57"/>
+      <c r="J196" s="58"/>
+      <c r="K196" s="58"/>
+      <c r="L196" s="58"/>
+      <c r="M196" s="58"/>
+      <c r="N196" s="58"/>
+    </row>
+    <row r="197" spans="2:14">
+      <c r="B197" s="44"/>
+      <c r="C197" s="52"/>
+      <c r="D197" s="52"/>
+      <c r="E197" s="57"/>
+      <c r="F197" s="57"/>
+      <c r="G197" s="57"/>
+      <c r="H197" s="57"/>
+      <c r="I197" s="57"/>
+      <c r="J197" s="58"/>
+      <c r="K197" s="58"/>
+      <c r="L197" s="58"/>
+      <c r="M197" s="58"/>
+      <c r="N197" s="58"/>
+    </row>
+    <row r="198" spans="2:14">
+      <c r="B198" s="44"/>
+      <c r="C198" s="52"/>
+      <c r="D198" s="52"/>
+      <c r="E198" s="57"/>
+      <c r="F198" s="57"/>
+      <c r="G198" s="57"/>
+      <c r="H198" s="57"/>
+      <c r="I198" s="57"/>
+      <c r="J198" s="58"/>
+      <c r="K198" s="58"/>
+      <c r="L198" s="58"/>
+      <c r="M198" s="58"/>
+      <c r="N198" s="58"/>
+    </row>
+    <row r="199" spans="2:14">
+      <c r="B199" s="44"/>
+      <c r="C199" s="52"/>
+      <c r="D199" s="52"/>
+      <c r="E199" s="57"/>
+      <c r="F199" s="57"/>
+      <c r="G199" s="57"/>
+      <c r="H199" s="57"/>
+      <c r="I199" s="57"/>
+      <c r="J199" s="58"/>
+      <c r="K199" s="58"/>
+      <c r="L199" s="58"/>
+      <c r="M199" s="58"/>
+      <c r="N199" s="58"/>
+    </row>
+    <row r="200" spans="2:14">
+      <c r="B200" s="44"/>
+      <c r="C200" s="52"/>
+      <c r="D200" s="52"/>
+      <c r="E200" s="57"/>
+      <c r="F200" s="57"/>
+      <c r="G200" s="57"/>
+      <c r="H200" s="57"/>
+      <c r="I200" s="57"/>
+      <c r="J200" s="58"/>
+      <c r="K200" s="58"/>
+      <c r="L200" s="58"/>
+      <c r="M200" s="58"/>
+      <c r="N200" s="58"/>
+    </row>
+    <row r="201" spans="2:14">
+      <c r="B201" s="44"/>
+      <c r="C201" s="52"/>
+      <c r="D201" s="52"/>
+      <c r="E201" s="57"/>
+      <c r="F201" s="57"/>
+      <c r="G201" s="57"/>
+      <c r="H201" s="57"/>
+      <c r="I201" s="57"/>
+      <c r="J201" s="58"/>
+      <c r="K201" s="58"/>
+      <c r="L201" s="58"/>
+      <c r="M201" s="58"/>
+      <c r="N201" s="58"/>
+    </row>
+    <row r="202" spans="2:14">
+      <c r="B202" s="44"/>
+      <c r="C202" s="52"/>
+      <c r="D202" s="52"/>
+      <c r="E202" s="57"/>
+      <c r="F202" s="57"/>
+      <c r="G202" s="57"/>
+      <c r="H202" s="57"/>
+      <c r="I202" s="57"/>
+      <c r="J202" s="58"/>
+      <c r="K202" s="58"/>
+      <c r="L202" s="58"/>
+      <c r="M202" s="58"/>
+      <c r="N202" s="58"/>
+    </row>
+    <row r="203" spans="2:14">
+      <c r="B203" s="44"/>
+      <c r="C203" s="52"/>
+      <c r="D203" s="52"/>
+      <c r="E203" s="57"/>
+      <c r="F203" s="57"/>
+      <c r="G203" s="57"/>
+      <c r="H203" s="57"/>
+      <c r="I203" s="57"/>
+      <c r="J203" s="58"/>
+      <c r="K203" s="58"/>
+      <c r="L203" s="58"/>
+      <c r="M203" s="58"/>
+      <c r="N203" s="58"/>
+    </row>
+    <row r="204" spans="2:14">
+      <c r="B204" s="44"/>
+      <c r="C204" s="52"/>
+      <c r="D204" s="52"/>
+      <c r="E204" s="57"/>
+      <c r="F204" s="57"/>
+      <c r="G204" s="57"/>
+      <c r="H204" s="57"/>
+      <c r="I204" s="57"/>
+      <c r="J204" s="58"/>
+      <c r="K204" s="58"/>
+      <c r="L204" s="58"/>
+      <c r="M204" s="58"/>
+      <c r="N204" s="58"/>
+    </row>
+    <row r="205" spans="2:14">
+      <c r="B205" s="44"/>
+      <c r="C205" s="52"/>
+      <c r="D205" s="52"/>
+      <c r="E205" s="57"/>
+      <c r="F205" s="57"/>
+      <c r="G205" s="57"/>
+      <c r="H205" s="57"/>
+      <c r="I205" s="57"/>
+      <c r="J205" s="58"/>
+      <c r="K205" s="58"/>
+      <c r="L205" s="58"/>
+      <c r="M205" s="58"/>
+      <c r="N205" s="58"/>
+    </row>
+    <row r="206" spans="2:14">
+      <c r="B206" s="44"/>
+      <c r="C206" s="52"/>
+      <c r="D206" s="52"/>
+      <c r="E206" s="57"/>
+      <c r="F206" s="57"/>
+      <c r="G206" s="57"/>
+      <c r="H206" s="57"/>
+      <c r="I206" s="57"/>
+      <c r="J206" s="58"/>
+      <c r="K206" s="58"/>
+      <c r="L206" s="58"/>
+      <c r="M206" s="58"/>
+      <c r="N206" s="58"/>
+    </row>
+    <row r="207" spans="2:14">
+      <c r="B207" s="44"/>
+      <c r="C207" s="56"/>
+      <c r="D207" s="56"/>
+      <c r="E207" s="59"/>
+      <c r="F207" s="59"/>
+      <c r="G207" s="59"/>
+      <c r="H207" s="59"/>
+      <c r="I207" s="60"/>
+      <c r="J207" s="59"/>
+      <c r="K207" s="58"/>
+      <c r="L207" s="58"/>
+      <c r="M207" s="58"/>
+      <c r="N207" s="58"/>
+    </row>
+    <row r="208" spans="2:14">
+      <c r="B208" s="44"/>
+      <c r="C208" s="52"/>
+      <c r="D208" s="52"/>
+      <c r="E208" s="57"/>
+      <c r="F208" s="57"/>
+      <c r="G208" s="57"/>
+      <c r="H208" s="57"/>
+      <c r="I208" s="57"/>
+      <c r="J208" s="61"/>
+      <c r="K208" s="58"/>
+      <c r="L208" s="58"/>
+      <c r="M208" s="58"/>
+      <c r="N208" s="58"/>
+    </row>
+    <row r="209" spans="1:14">
+      <c r="B209" s="44"/>
+      <c r="C209" s="52"/>
+      <c r="D209" s="52"/>
+      <c r="E209" s="57"/>
+      <c r="F209" s="57"/>
+      <c r="G209" s="57"/>
+      <c r="H209" s="57"/>
+      <c r="I209" s="57"/>
+      <c r="J209" s="61"/>
+      <c r="K209" s="58"/>
+      <c r="L209" s="58"/>
+      <c r="M209" s="58"/>
+      <c r="N209" s="58"/>
+    </row>
+    <row r="210" spans="1:14">
+      <c r="B210" s="44"/>
+      <c r="C210" s="52"/>
+      <c r="D210" s="52"/>
+      <c r="E210" s="57"/>
+      <c r="F210" s="57"/>
+      <c r="G210" s="57"/>
+      <c r="H210" s="57"/>
+      <c r="I210" s="57"/>
+      <c r="J210" s="61"/>
+      <c r="K210" s="58"/>
+      <c r="L210" s="58"/>
+      <c r="M210" s="58"/>
+      <c r="N210" s="58"/>
+    </row>
+    <row r="211" spans="1:14">
+      <c r="B211" s="44"/>
+      <c r="C211" s="52"/>
+      <c r="D211" s="52"/>
+      <c r="E211" s="57"/>
+      <c r="F211" s="57"/>
+      <c r="G211" s="57"/>
+      <c r="H211" s="57"/>
+      <c r="I211" s="57"/>
+      <c r="J211" s="61"/>
+      <c r="K211" s="58"/>
+      <c r="L211" s="58"/>
+      <c r="M211" s="58"/>
+      <c r="N211" s="58"/>
+    </row>
+    <row r="212" spans="1:14">
+      <c r="J212" s="35"/>
+    </row>
+    <row r="214" spans="1:14">
+      <c r="A214" s="5"/>
+      <c r="B214" s="62"/>
+      <c r="C214" s="55"/>
+      <c r="D214" s="55"/>
+      <c r="E214" s="55"/>
+      <c r="F214" s="55"/>
+      <c r="G214" s="55"/>
+      <c r="H214" s="55"/>
+      <c r="I214" s="55"/>
+      <c r="J214" s="55"/>
+    </row>
+    <row r="215" spans="1:14">
+      <c r="B215" s="44"/>
+      <c r="C215" s="43"/>
+      <c r="D215" s="43"/>
+      <c r="E215" s="43"/>
+      <c r="G215" s="43"/>
+      <c r="H215" s="43"/>
+      <c r="I215" s="43"/>
+      <c r="J215" s="64"/>
+    </row>
+    <row r="216" spans="1:14">
+      <c r="B216" s="44"/>
+      <c r="C216" s="43"/>
+      <c r="D216" s="43"/>
+      <c r="E216" s="43"/>
+      <c r="F216" s="43"/>
+      <c r="G216" s="43"/>
+      <c r="H216" s="43"/>
+      <c r="I216" s="43"/>
+      <c r="J216" s="64"/>
+    </row>
+    <row r="217" spans="1:14">
+      <c r="B217" s="44"/>
+      <c r="C217" s="43"/>
+      <c r="D217" s="43"/>
+      <c r="E217" s="43"/>
+      <c r="F217" s="43"/>
+      <c r="G217" s="43"/>
+      <c r="H217" s="43"/>
+      <c r="I217" s="43"/>
+      <c r="J217" s="64"/>
+    </row>
+    <row r="218" spans="1:14">
+      <c r="B218" s="44"/>
+      <c r="C218" s="43"/>
+      <c r="D218" s="43"/>
+      <c r="E218" s="43"/>
+      <c r="F218" s="43"/>
+      <c r="G218" s="43"/>
+      <c r="H218" s="43"/>
+      <c r="I218" s="43"/>
+      <c r="J218" s="64"/>
+    </row>
+    <row r="219" spans="1:14">
+      <c r="B219" s="44"/>
+      <c r="C219" s="43"/>
+      <c r="D219" s="43"/>
+      <c r="E219" s="43"/>
+      <c r="F219" s="43"/>
+      <c r="G219" s="43"/>
+      <c r="H219" s="43"/>
+      <c r="I219" s="43"/>
+      <c r="J219" s="64"/>
+    </row>
+    <row r="222" spans="1:14">
+      <c r="A222" s="5"/>
+      <c r="B222" s="62"/>
+      <c r="C222" s="55"/>
+    </row>
+    <row r="223" spans="1:14">
+      <c r="B223" s="44"/>
+      <c r="C223" s="64"/>
+    </row>
+    <row r="224" spans="1:14">
+      <c r="B224" s="44"/>
+      <c r="C224" s="43"/>
+    </row>
+    <row r="225" spans="1:8">
+      <c r="B225" s="44"/>
+      <c r="C225" s="43"/>
+    </row>
+    <row r="226" spans="1:8">
+      <c r="B226" s="44"/>
+      <c r="C226" s="43"/>
+    </row>
+    <row r="227" spans="1:8">
+      <c r="B227" s="44"/>
+      <c r="C227" s="43"/>
+    </row>
+    <row r="228" spans="1:8">
+      <c r="B228" s="44"/>
+      <c r="C228" s="43"/>
+    </row>
+    <row r="229" spans="1:8">
+      <c r="B229" s="44"/>
+      <c r="C229" s="43"/>
+    </row>
+    <row r="232" spans="1:8">
+      <c r="A232" s="5"/>
+      <c r="B232" s="62"/>
+      <c r="C232" s="55"/>
+      <c r="D232" s="55"/>
+      <c r="E232" s="55"/>
+      <c r="F232" s="55"/>
+      <c r="G232" s="55"/>
+      <c r="H232" s="55"/>
+    </row>
+    <row r="233" spans="1:8">
+      <c r="B233" s="44"/>
+      <c r="C233" s="43"/>
+      <c r="D233" s="43"/>
+      <c r="E233" s="43"/>
+      <c r="F233" s="43"/>
+      <c r="G233" s="43"/>
+      <c r="H233" s="43"/>
+    </row>
+    <row r="234" spans="1:8">
+      <c r="B234" s="44"/>
+      <c r="C234" s="43"/>
+      <c r="D234" s="43"/>
+      <c r="E234" s="43"/>
+      <c r="F234" s="43"/>
+      <c r="G234" s="43"/>
+      <c r="H234" s="43"/>
+    </row>
+    <row r="235" spans="1:8">
+      <c r="B235" s="44"/>
+      <c r="C235" s="43"/>
+      <c r="D235" s="43"/>
+      <c r="E235" s="43"/>
+      <c r="F235" s="43"/>
+      <c r="G235" s="43"/>
+      <c r="H235" s="43"/>
+    </row>
+    <row r="236" spans="1:8">
+      <c r="B236" s="44"/>
+      <c r="C236" s="43"/>
+      <c r="D236" s="43"/>
+      <c r="E236" s="43"/>
+      <c r="F236" s="43"/>
+      <c r="G236" s="43"/>
+      <c r="H236" s="43"/>
+    </row>
+    <row r="241" spans="3:7">
+      <c r="C241" s="36"/>
+      <c r="D241" s="36"/>
+      <c r="E241" s="36"/>
+      <c r="F241" s="36"/>
+      <c r="G241" s="36"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B107">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"No Committee"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"No Committee"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>"No Committee"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B86">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"No Committee"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B147">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"No Committee"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B169">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="B107 B65 B44 B86 B149 B170">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"No Committee"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>